<commit_message>
Lot of updates since last push
</commit_message>
<xml_diff>
--- a/StrainMenu Creator/bin/Release/Generated.xlsx
+++ b/StrainMenu Creator/bin/Release/Generated.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Joe\source\repos\StrainMenu Creator\StrainMenu Creator\bin\Release\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{762B81EB-5D92-4D3F-A702-2B49FB8EB9CD}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AB8DD8E-617A-4FFC-BF2C-C88608238C06}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" xr2:uid="{BBEC57AF-E876-4348-A0BF-72133E8375A3}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="48">
   <si>
     <t>Strain:</t>
   </si>
@@ -60,112 +60,115 @@
     <t>Bulk Grams</t>
   </si>
   <si>
-    <t>OG18</t>
-  </si>
-  <si>
-    <t>Zkittlez</t>
-  </si>
-  <si>
-    <t>Lemon G</t>
-  </si>
-  <si>
-    <t>The Mountain</t>
-  </si>
-  <si>
-    <t>Blue Dream</t>
-  </si>
-  <si>
-    <t>Powder Puff</t>
-  </si>
-  <si>
-    <t>Lavender</t>
-  </si>
-  <si>
-    <t>Kosh Dawg</t>
-  </si>
-  <si>
-    <t>Orange ACDC</t>
-  </si>
-  <si>
-    <t>Grape Cheesecake</t>
-  </si>
-  <si>
-    <t>Mega Jackpot</t>
-  </si>
-  <si>
-    <t>Green Goddess</t>
-  </si>
-  <si>
-    <t>Banana Split</t>
-  </si>
-  <si>
-    <t>Adak</t>
-  </si>
-  <si>
-    <t>CBD Nordle</t>
-  </si>
-  <si>
-    <t>Dosido</t>
-  </si>
-  <si>
-    <t>Jack &amp; Cheese</t>
-  </si>
-  <si>
-    <t>Big Smooth</t>
-  </si>
-  <si>
-    <t>key Lime Pie</t>
-  </si>
-  <si>
-    <t>Grape Valley Kush</t>
-  </si>
-  <si>
-    <t>Mendo Breath</t>
-  </si>
-  <si>
-    <t>Lezberado</t>
-  </si>
-  <si>
-    <t>Snowman Cookies</t>
-  </si>
-  <si>
-    <t>Strawberry Banana</t>
-  </si>
-  <si>
-    <t>Ogre</t>
-  </si>
-  <si>
-    <t>Poison Sunset</t>
-  </si>
-  <si>
-    <t>Cookies &amp; Cream</t>
-  </si>
-  <si>
-    <t>Black Diamond</t>
-  </si>
-  <si>
-    <t>Afgoo</t>
-  </si>
-  <si>
-    <t>Junior Mints</t>
-  </si>
-  <si>
-    <t>Black Jack</t>
-  </si>
-  <si>
-    <t>Yesterdays Paper</t>
-  </si>
-  <si>
-    <t>White 99</t>
-  </si>
-  <si>
-    <t>Sweet Thang #7</t>
-  </si>
-  <si>
-    <t>Hawaiian Dutch</t>
-  </si>
-  <si>
-    <t>J1</t>
+    <t>1: OG18</t>
+  </si>
+  <si>
+    <t>2: Zkittlez</t>
+  </si>
+  <si>
+    <t>3: Lemon G</t>
+  </si>
+  <si>
+    <t>4: The Mountain</t>
+  </si>
+  <si>
+    <t>5: Blue Dream</t>
+  </si>
+  <si>
+    <t>6: Powder Puff</t>
+  </si>
+  <si>
+    <t>7: Lavender</t>
+  </si>
+  <si>
+    <t>8: Kosh Dawg</t>
+  </si>
+  <si>
+    <t>9: Powder Puff</t>
+  </si>
+  <si>
+    <t>10: Orange ACDC</t>
+  </si>
+  <si>
+    <t>11: Grape Cheesecake</t>
+  </si>
+  <si>
+    <t>12: Mega Jackpot</t>
+  </si>
+  <si>
+    <t>13: Green Goddess</t>
+  </si>
+  <si>
+    <t>14: Banana Split</t>
+  </si>
+  <si>
+    <t>15: Adak</t>
+  </si>
+  <si>
+    <t>16: CBD Nordle</t>
+  </si>
+  <si>
+    <t>17: Dosido</t>
+  </si>
+  <si>
+    <t>18: Jack &amp; Cheese</t>
+  </si>
+  <si>
+    <t>19: Big Smooth</t>
+  </si>
+  <si>
+    <t>20: key Lime Pie</t>
+  </si>
+  <si>
+    <t>21: Grape Valley Kush</t>
+  </si>
+  <si>
+    <t>22: Mendo Breath</t>
+  </si>
+  <si>
+    <t>23: Lezberado</t>
+  </si>
+  <si>
+    <t>24: Snowman Cookies</t>
+  </si>
+  <si>
+    <t>25: Strawberry Banana</t>
+  </si>
+  <si>
+    <t>26: Ogre</t>
+  </si>
+  <si>
+    <t>27: Poison Sunset</t>
+  </si>
+  <si>
+    <t>28: Cookies &amp; Cream</t>
+  </si>
+  <si>
+    <t>29: Black Diamond</t>
+  </si>
+  <si>
+    <t>30: Afgoo</t>
+  </si>
+  <si>
+    <t>31: Junior Mints</t>
+  </si>
+  <si>
+    <t>32: Black Jack</t>
+  </si>
+  <si>
+    <t>33: Yesterdays Paper</t>
+  </si>
+  <si>
+    <t>34: White 99</t>
+  </si>
+  <si>
+    <t>35: Sweet Thang #7</t>
+  </si>
+  <si>
+    <t>36: Hawaiian Dutch</t>
+  </si>
+  <si>
+    <t>37: J1</t>
   </si>
 </sst>
 </file>
@@ -1120,7 +1123,7 @@
       <c r="F4" s="7"/>
       <c r="G4" s="7"/>
       <c r="H4" s="79" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="I4" s="80">
         <v>9.6</v>
@@ -1153,7 +1156,7 @@
       <c r="F5" s="8"/>
       <c r="G5" s="8"/>
       <c r="H5" s="51" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="I5" s="59">
         <v>9.6</v>
@@ -1186,7 +1189,7 @@
       <c r="F6" s="7"/>
       <c r="G6" s="7"/>
       <c r="H6" s="43" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="I6" s="83">
         <v>9.6</v>
@@ -1219,7 +1222,7 @@
       <c r="F7" s="7"/>
       <c r="G7" s="7"/>
       <c r="H7" s="47" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="I7" s="72">
         <v>12</v>
@@ -1252,7 +1255,7 @@
       <c r="F8" s="7"/>
       <c r="G8" s="7"/>
       <c r="H8" s="60" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="I8" s="84">
         <v>12</v>
@@ -1285,7 +1288,7 @@
       <c r="F9" s="7"/>
       <c r="G9" s="7"/>
       <c r="H9" s="47" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="I9" s="72">
         <v>12</v>
@@ -1318,7 +1321,7 @@
       <c r="F10" s="7"/>
       <c r="G10" s="7"/>
       <c r="H10" s="43" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="I10" s="44">
         <v>12</v>
@@ -1351,7 +1354,7 @@
       <c r="F11" s="7"/>
       <c r="G11" s="7"/>
       <c r="H11" s="51" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="I11" s="52">
         <v>12</v>
@@ -1370,7 +1373,7 @@
     <row r="12" spans="1:15" ht="36" x14ac:dyDescent="0.5">
       <c r="A12" s="2"/>
       <c r="B12" s="47" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="C12" s="48">
         <v>6</v>
@@ -1384,7 +1387,7 @@
       <c r="F12" s="7"/>
       <c r="G12" s="7"/>
       <c r="H12" s="35" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="I12" s="36">
         <v>12</v>
@@ -1403,7 +1406,7 @@
     <row r="13" spans="1:15" ht="36" x14ac:dyDescent="0.5">
       <c r="A13" s="2"/>
       <c r="B13" s="55" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C13" s="56">
         <v>6</v>
@@ -1417,7 +1420,7 @@
       <c r="F13" s="7"/>
       <c r="G13" s="7"/>
       <c r="H13" s="51" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="I13" s="59">
         <v>12</v>
@@ -1436,7 +1439,7 @@
     <row r="14" spans="1:15" ht="36" x14ac:dyDescent="0.5">
       <c r="A14" s="2"/>
       <c r="B14" s="39" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C14" s="40">
         <v>7.2</v>
@@ -1450,7 +1453,7 @@
       <c r="F14" s="7"/>
       <c r="G14" s="7"/>
       <c r="H14" s="35" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="I14" s="86">
         <v>12</v>
@@ -1469,7 +1472,7 @@
     <row r="15" spans="1:15" ht="36" x14ac:dyDescent="0.5">
       <c r="A15" s="2"/>
       <c r="B15" s="43" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C15" s="44">
         <v>7.2</v>
@@ -1483,7 +1486,7 @@
       <c r="F15" s="7"/>
       <c r="G15" s="7"/>
       <c r="H15" s="47" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="I15" s="72">
         <v>12</v>
@@ -1502,7 +1505,7 @@
     <row r="16" spans="1:15" ht="36" x14ac:dyDescent="0.5">
       <c r="A16" s="2"/>
       <c r="B16" s="51" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C16" s="59">
         <v>7.2</v>
@@ -1516,7 +1519,7 @@
       <c r="F16" s="7"/>
       <c r="G16" s="7"/>
       <c r="H16" s="43" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="I16" s="83">
         <v>12</v>
@@ -1535,7 +1538,7 @@
     <row r="17" spans="1:15" ht="36" x14ac:dyDescent="0.5">
       <c r="A17" s="2"/>
       <c r="B17" s="60" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C17" s="61">
         <v>9.6</v>
@@ -1549,7 +1552,7 @@
       <c r="F17" s="7"/>
       <c r="G17" s="7"/>
       <c r="H17" s="47" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="I17" s="72">
         <v>12</v>
@@ -1568,7 +1571,7 @@
     <row r="18" spans="1:15" ht="36" x14ac:dyDescent="0.5">
       <c r="A18" s="2"/>
       <c r="B18" s="51" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C18" s="59">
         <v>9.6</v>
@@ -1582,7 +1585,7 @@
       <c r="F18" s="7"/>
       <c r="G18" s="7"/>
       <c r="H18" s="43" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="I18" s="83">
         <v>12</v>
@@ -1601,7 +1604,7 @@
     <row r="19" spans="1:15" ht="36" x14ac:dyDescent="0.5">
       <c r="A19" s="2"/>
       <c r="B19" s="55" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C19" s="69">
         <v>9.6</v>
@@ -1615,7 +1618,7 @@
       <c r="F19" s="7"/>
       <c r="G19" s="7"/>
       <c r="H19" s="64" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="I19" s="65">
         <v>14.4</v>
@@ -1634,7 +1637,7 @@
     <row r="20" spans="1:15" ht="36" x14ac:dyDescent="0.5">
       <c r="A20" s="2"/>
       <c r="B20" s="47" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C20" s="72">
         <v>9.6</v>
@@ -1648,7 +1651,7 @@
       <c r="F20" s="7"/>
       <c r="G20" s="7"/>
       <c r="H20" s="43" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="I20" s="83">
         <v>14.4</v>
@@ -1667,7 +1670,7 @@
     <row r="21" spans="1:15" ht="36" x14ac:dyDescent="0.5">
       <c r="A21" s="3"/>
       <c r="B21" s="43" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C21" s="44">
         <v>9.6</v>
@@ -1692,7 +1695,7 @@
     <row r="22" spans="1:15" ht="36" x14ac:dyDescent="0.4">
       <c r="A22" s="3"/>
       <c r="B22" s="47" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C22" s="72">
         <v>9.6</v>
@@ -1717,7 +1720,7 @@
     <row r="23" spans="1:15" ht="36" x14ac:dyDescent="0.45">
       <c r="A23" s="3"/>
       <c r="B23" s="75" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C23" s="76">
         <v>9.6</v>

</xml_diff>